<commit_message>
Add new and updated project files.
</commit_message>
<xml_diff>
--- a/data/growth.xlsx
+++ b/data/growth.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,14 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <r>
       <rPr>
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>ABC</t>
+      <t>CRK</t>
     </r>
   </si>
   <si>
@@ -35,115 +35,27 @@
         <sz val="11.5"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>AmerisourceBergen Corp</t>
+      <t>Comstock Resources Inc</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>18.98B</t>
-    </r>
+    <t>BGD</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>3.47K%</t>
-    </r>
+    <t>Nothing</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>MGM</t>
-    </r>
+    <t>FDS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>MGM Resorts International</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>8.932B</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>3.18K%</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>ALGN</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Align Technology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> Inc</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>19.80B</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>2.06K%</t>
-    </r>
+    <t>Nothing  1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0."/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -153,6 +65,20 @@
     <font>
       <sz val="11.5"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,19 +113,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,23 +462,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="37.5" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="44.83203125" customWidth="1"/>
+    <col min="3" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,57 +484,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2">
-        <v>93.33</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>4.88</v>
+      </c>
+      <c r="D1" s="1">
+        <v>1.131</v>
+      </c>
+      <c r="E1" s="3">
+        <v>0.15379999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="60">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <v>18.11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>251.41</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14"/>
-    <row r="5" spans="1:5" ht="14"/>
-    <row r="6" spans="1:5" ht="14"/>
-    <row r="7" spans="1:5" ht="14"/>
-    <row r="8" spans="1:5" ht="14"/>
-    <row r="9" spans="1:5" ht="14"/>
   </sheetData>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.79166666666666696" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add updated data files.
</commit_message>
<xml_diff>
--- a/data/growth.xlsx
+++ b/data/growth.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,64 +19,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>CRK</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.5"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Comstock Resources Inc</t>
-    </r>
-  </si>
-  <si>
-    <t>BGD</t>
-  </si>
-  <si>
-    <t>Nothing</t>
-  </si>
-  <si>
-    <t>FDS</t>
-  </si>
-  <si>
-    <t>Nothing  1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>AMP</t>
+  </si>
+  <si>
+    <t>Ameriprise Financial Inc</t>
+  </si>
+  <si>
+    <t>15.73B</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>MetLife Inc</t>
+  </si>
+  <si>
+    <t>29.40B</t>
+  </si>
+  <si>
+    <t>AIG</t>
+  </si>
+  <si>
+    <t>American International Group Inc</t>
+  </si>
+  <si>
+    <t>23.80B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11.5"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -89,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,42 +76,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -462,74 +415,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="44.83203125" customWidth="1"/>
     <col min="3" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2">
-        <v>4.88</v>
-      </c>
-      <c r="D1" s="1">
-        <v>1.131</v>
-      </c>
-      <c r="E1" s="3">
-        <v>0.15379999999999999</v>
+      <c r="C1">
+        <v>128.54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4.6310000000000002</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>32.39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.3929999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
+        <v>27.63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.64</v>
       </c>
     </row>
+    <row r="7" spans="1:5" ht="14" customHeight="1"/>
+    <row r="9" spans="1:5" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="1.25" right="1.25" top="1" bottom="0.79166666666666696" header="0.25" footer="0.25"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>